<commit_message>
incluindo many to many
</commit_message>
<xml_diff>
--- a/tabelas.xlsx
+++ b/tabelas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee5e4464036fb731/Programming/Python/loja-bike/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{6E85F2BB-2271-4558-B0EE-41A9E4A59795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8F31BF7-98E9-417F-A0FE-067DC7BCAD7F}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{6E85F2BB-2271-4558-B0EE-41A9E4A59795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{303B5864-63C9-44A0-8224-C9C587C6691E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{712B301B-4A98-4648-9917-376F3A3A0935}"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{712B301B-4A98-4648-9917-376F3A3A0935}"/>
   </bookViews>
   <sheets>
     <sheet name="Produtos" sheetId="1" r:id="rId1"/>
@@ -116,13 +116,13 @@
     <t>id_produto</t>
   </si>
   <si>
-    <t>quantidade</t>
-  </si>
-  <si>
     <t>nome</t>
   </si>
   <si>
     <t>idade</t>
+  </si>
+  <si>
+    <t>id_venda</t>
   </si>
 </sst>
 </file>
@@ -596,7 +596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9715C11-DB12-43BC-AEDE-362ECA2B13C9}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -607,10 +607,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
         <v>27</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -660,10 +660,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECD29CB-1A73-4DEC-9E82-589C722A9E9C}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,13 +674,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -691,15 +691,15 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -707,21 +707,21 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -732,10 +732,21 @@
         <v>4</v>
       </c>
       <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>1</v>
+      <c r="C7">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>